<commit_message>
change all width to 8mil
</commit_message>
<xml_diff>
--- a/stm32f103_fc.xlsx
+++ b/stm32f103_fc.xlsx
@@ -309,7 +309,7 @@
     <t>1X2-3.5MM</t>
   </si>
   <si>
-    <t>PYRO1, PYRO2</t>
+    <t>PY1, PY2</t>
   </si>
   <si>
     <t>3.5mm Terminal block</t>
@@ -507,7 +507,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -515,6 +515,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -531,7 +536,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,8 +555,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -563,6 +574,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -576,7 +609,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -585,7 +618,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,43 +627,28 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,28 +657,58 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -670,68 +718,74 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -751,8 +805,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -771,10 +827,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -951,11 +1007,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -964,7 +1023,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -979,12 +1038,12 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -1241,10 +1300,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1535,7 +1594,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1816,7 +1875,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:L31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1831,8 +1890,8 @@
     <col min="7" max="7" width="11.8516" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.67188" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.6719" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="86.5234" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="86.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.35156" style="1" customWidth="1"/>
     <col min="13" max="256" width="8.35156" style="1" customWidth="1"/>
   </cols>
@@ -1841,979 +1900,979 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="I2" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="J2" t="s" s="4">
+      <c r="J2" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="K2" t="s" s="5">
         <v>11</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="L2" t="s" s="5">
         <v>12</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="5">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" t="s" s="7">
+      <c r="B3" s="8"/>
+      <c r="C3" t="s" s="9">
         <v>13</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="E3" t="s" s="9">
         <v>15</v>
       </c>
-      <c r="F3" t="s" s="7">
+      <c r="F3" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="G3" t="s" s="7">
+      <c r="G3" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" t="s" s="7">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
+      <c r="K3" t="s" s="9">
         <v>18</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="12">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="11">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" t="s" s="13">
+      <c r="B4" s="14"/>
+      <c r="C4" t="s" s="15">
         <v>19</v>
       </c>
-      <c r="D4" t="s" s="13">
+      <c r="D4" t="s" s="15">
         <v>20</v>
       </c>
-      <c r="E4" t="s" s="13">
+      <c r="E4" t="s" s="15">
         <v>21</v>
       </c>
-      <c r="F4" t="s" s="13">
+      <c r="F4" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
-      <c r="K4" t="s" s="13">
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
+      <c r="K4" t="s" s="15">
         <v>22</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="11">
+      <c r="A5" s="13">
         <v>1</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" t="s" s="13">
+      <c r="B5" s="14"/>
+      <c r="C5" t="s" s="15">
         <v>23</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" t="s" s="15">
         <v>24</v>
       </c>
-      <c r="E5" t="s" s="13">
+      <c r="E5" t="s" s="15">
         <v>25</v>
       </c>
-      <c r="F5" t="s" s="13">
+      <c r="F5" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" t="s" s="13">
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" t="s" s="15">
         <v>22</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="11">
+      <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" t="s" s="13">
+      <c r="B6" s="14"/>
+      <c r="C6" t="s" s="15">
         <v>26</v>
       </c>
-      <c r="D6" t="s" s="13">
+      <c r="D6" t="s" s="15">
         <v>27</v>
       </c>
-      <c r="E6" t="s" s="13">
+      <c r="E6" t="s" s="15">
         <v>28</v>
       </c>
-      <c r="F6" t="s" s="13">
+      <c r="F6" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="G6" t="s" s="13">
+      <c r="G6" t="s" s="15">
         <v>29</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
-      <c r="K6" t="s" s="13">
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
+      <c r="K6" t="s" s="15">
         <v>22</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="11">
+      <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" t="s" s="13">
+      <c r="B7" s="14"/>
+      <c r="C7" t="s" s="15">
         <v>30</v>
       </c>
-      <c r="D7" t="s" s="13">
+      <c r="D7" t="s" s="15">
         <v>31</v>
       </c>
-      <c r="E7" t="s" s="13">
+      <c r="E7" t="s" s="15">
         <v>32</v>
       </c>
-      <c r="F7" t="s" s="13">
+      <c r="F7" t="s" s="15">
         <v>33</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
-      <c r="K7" t="s" s="13">
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" t="s" s="15">
         <v>34</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="11">
+      <c r="A8" s="13">
         <v>1</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" t="s" s="13">
+      <c r="B8" s="14"/>
+      <c r="C8" t="s" s="15">
         <v>35</v>
       </c>
-      <c r="D8" t="s" s="13">
+      <c r="D8" t="s" s="15">
         <v>36</v>
       </c>
-      <c r="E8" t="s" s="13">
+      <c r="E8" t="s" s="15">
         <v>37</v>
       </c>
-      <c r="F8" t="s" s="13">
+      <c r="F8" t="s" s="15">
         <v>38</v>
       </c>
-      <c r="G8" t="s" s="13">
+      <c r="G8" t="s" s="15">
         <v>39</v>
       </c>
-      <c r="H8" t="s" s="13">
+      <c r="H8" t="s" s="15">
         <v>40</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
-      <c r="K8" t="s" s="13">
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
+      <c r="K8" t="s" s="15">
         <v>41</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="11">
+      <c r="A9" s="13">
         <v>5</v>
       </c>
-      <c r="B9" t="s" s="17">
+      <c r="B9" t="s" s="19">
         <v>42</v>
       </c>
-      <c r="C9" t="s" s="13">
+      <c r="C9" t="s" s="15">
         <v>43</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="18">
         <v>402</v>
       </c>
-      <c r="E9" t="s" s="13">
+      <c r="E9" t="s" s="15">
         <v>44</v>
       </c>
-      <c r="F9" t="s" s="13">
+      <c r="F9" t="s" s="15">
         <v>45</v>
       </c>
-      <c r="G9" t="s" s="13">
+      <c r="G9" t="s" s="15">
         <v>46</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" t="s" s="18">
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" t="s" s="20">
         <v>42</v>
       </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="16">
+      <c r="K9" s="16"/>
+      <c r="L9" s="18">
         <f>A2:A31*5</f>
         <v>25</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="11">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
-      <c r="B10" t="s" s="17">
+      <c r="B10" t="s" s="19">
         <v>42</v>
       </c>
-      <c r="C10" t="s" s="13">
+      <c r="C10" t="s" s="15">
         <v>47</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="18">
         <v>603</v>
       </c>
-      <c r="E10" t="s" s="13">
+      <c r="E10" t="s" s="15">
         <v>48</v>
       </c>
-      <c r="F10" t="s" s="13">
+      <c r="F10" t="s" s="15">
         <v>45</v>
       </c>
-      <c r="G10" t="s" s="13">
+      <c r="G10" t="s" s="15">
         <v>49</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" t="s" s="18">
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" t="s" s="20">
         <v>42</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="16">
+      <c r="K10" s="16"/>
+      <c r="L10" s="18">
         <f>A2:A31*5</f>
         <v>15</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11">
+      <c r="A11" s="13">
         <v>1</v>
       </c>
-      <c r="B11" t="s" s="17">
+      <c r="B11" t="s" s="19">
         <v>50</v>
       </c>
-      <c r="C11" t="s" s="13">
+      <c r="C11" t="s" s="15">
         <v>51</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="18">
         <v>603</v>
       </c>
-      <c r="E11" t="s" s="13">
+      <c r="E11" t="s" s="15">
         <v>52</v>
       </c>
-      <c r="F11" t="s" s="13">
+      <c r="F11" t="s" s="15">
         <v>53</v>
       </c>
-      <c r="G11" t="s" s="13">
+      <c r="G11" t="s" s="15">
         <v>54</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" t="s" s="18">
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" t="s" s="20">
         <v>50</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="16">
+      <c r="K11" s="16"/>
+      <c r="L11" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="11">
+      <c r="A12" s="13">
         <v>2</v>
       </c>
-      <c r="B12" t="s" s="17">
+      <c r="B12" t="s" s="19">
         <v>55</v>
       </c>
-      <c r="C12" t="s" s="13">
+      <c r="C12" t="s" s="15">
         <v>56</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="18">
         <v>603</v>
       </c>
-      <c r="E12" t="s" s="13">
+      <c r="E12" t="s" s="15">
         <v>57</v>
       </c>
-      <c r="F12" t="s" s="13">
+      <c r="F12" t="s" s="15">
         <v>58</v>
       </c>
-      <c r="G12" t="s" s="13">
+      <c r="G12" t="s" s="15">
         <v>59</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" t="s" s="18">
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" t="s" s="20">
         <v>55</v>
       </c>
-      <c r="K12" s="14"/>
-      <c r="L12" s="16">
+      <c r="K12" s="16"/>
+      <c r="L12" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="11">
+      <c r="A13" s="13">
         <v>1</v>
       </c>
-      <c r="B13" t="s" s="17">
+      <c r="B13" t="s" s="19">
         <v>60</v>
       </c>
-      <c r="C13" t="s" s="13">
+      <c r="C13" t="s" s="15">
         <v>47</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="18">
         <v>603</v>
       </c>
-      <c r="E13" t="s" s="13">
+      <c r="E13" t="s" s="15">
         <v>61</v>
       </c>
-      <c r="F13" t="s" s="13">
+      <c r="F13" t="s" s="15">
         <v>45</v>
       </c>
-      <c r="G13" t="s" s="13">
+      <c r="G13" t="s" s="15">
         <v>49</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" t="s" s="18">
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" t="s" s="20">
         <v>42</v>
       </c>
-      <c r="K13" s="14"/>
-      <c r="L13" s="16">
+      <c r="K13" s="16"/>
+      <c r="L13" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="11">
+      <c r="A14" s="13">
         <v>2</v>
       </c>
-      <c r="B14" t="s" s="17">
+      <c r="B14" t="s" s="19">
         <v>62</v>
       </c>
-      <c r="C14" t="s" s="13">
+      <c r="C14" t="s" s="15">
         <v>63</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="18">
         <v>603</v>
       </c>
-      <c r="E14" t="s" s="13">
+      <c r="E14" t="s" s="15">
         <v>64</v>
       </c>
-      <c r="F14" t="s" s="13">
+      <c r="F14" t="s" s="15">
         <v>65</v>
       </c>
-      <c r="G14" t="s" s="13">
+      <c r="G14" t="s" s="15">
         <v>66</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" t="s" s="18">
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" t="s" s="20">
         <v>62</v>
       </c>
-      <c r="K14" s="14"/>
-      <c r="L14" s="16">
+      <c r="K14" s="16"/>
+      <c r="L14" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="11">
+      <c r="A15" s="13">
         <v>2</v>
       </c>
-      <c r="B15" t="s" s="17">
+      <c r="B15" t="s" s="19">
         <v>67</v>
       </c>
-      <c r="C15" t="s" s="13">
+      <c r="C15" t="s" s="15">
         <v>68</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="18">
         <v>603</v>
       </c>
-      <c r="E15" t="s" s="13">
+      <c r="E15" t="s" s="15">
         <v>69</v>
       </c>
-      <c r="F15" t="s" s="13">
+      <c r="F15" t="s" s="15">
         <v>70</v>
       </c>
-      <c r="G15" t="s" s="13">
+      <c r="G15" t="s" s="15">
         <v>71</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" t="s" s="18">
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" t="s" s="20">
         <v>67</v>
       </c>
-      <c r="K15" s="14"/>
-      <c r="L15" s="16">
+      <c r="K15" s="16"/>
+      <c r="L15" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="11">
+      <c r="A16" s="13">
         <v>1</v>
       </c>
-      <c r="B16" t="s" s="17">
+      <c r="B16" t="s" s="19">
         <v>72</v>
       </c>
-      <c r="C16" t="s" s="13">
+      <c r="C16" t="s" s="15">
         <v>73</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="18">
         <v>603</v>
       </c>
-      <c r="E16" t="s" s="13">
+      <c r="E16" t="s" s="15">
         <v>74</v>
       </c>
-      <c r="F16" t="s" s="13">
+      <c r="F16" t="s" s="15">
         <v>75</v>
       </c>
-      <c r="G16" t="s" s="13">
+      <c r="G16" t="s" s="15">
         <v>76</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" t="s" s="18">
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="K16" s="14"/>
-      <c r="L16" s="16">
+      <c r="K16" s="16"/>
+      <c r="L16" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="11">
+      <c r="A17" s="13">
         <v>1</v>
       </c>
-      <c r="B17" t="s" s="17">
+      <c r="B17" t="s" s="19">
         <v>77</v>
       </c>
-      <c r="C17" t="s" s="13">
+      <c r="C17" t="s" s="15">
         <v>78</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="18">
         <v>603</v>
       </c>
-      <c r="E17" t="s" s="13">
+      <c r="E17" t="s" s="15">
         <v>79</v>
       </c>
-      <c r="F17" t="s" s="13">
+      <c r="F17" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="G17" t="s" s="13">
+      <c r="G17" t="s" s="15">
         <v>81</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" t="s" s="18">
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" t="s" s="20">
         <v>77</v>
       </c>
-      <c r="K17" s="14"/>
-      <c r="L17" s="16">
+      <c r="K17" s="16"/>
+      <c r="L17" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="11">
+      <c r="A18" s="13">
         <v>2</v>
       </c>
-      <c r="B18" t="s" s="17">
+      <c r="B18" t="s" s="19">
         <v>82</v>
       </c>
-      <c r="C18" t="s" s="13">
+      <c r="C18" t="s" s="15">
         <v>83</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="18">
         <v>603</v>
       </c>
-      <c r="E18" t="s" s="13">
+      <c r="E18" t="s" s="15">
         <v>84</v>
       </c>
-      <c r="F18" t="s" s="13">
+      <c r="F18" t="s" s="15">
         <v>85</v>
       </c>
-      <c r="G18" t="s" s="13">
+      <c r="G18" t="s" s="15">
         <v>86</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" t="s" s="18">
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" t="s" s="20">
         <v>82</v>
       </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="16">
+      <c r="K18" s="16"/>
+      <c r="L18" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="11">
+      <c r="A19" s="13">
         <v>2</v>
       </c>
-      <c r="B19" t="s" s="17">
+      <c r="B19" t="s" s="19">
         <v>87</v>
       </c>
-      <c r="C19" t="s" s="13">
+      <c r="C19" t="s" s="15">
         <v>13</v>
       </c>
-      <c r="D19" t="s" s="13">
+      <c r="D19" t="s" s="15">
         <v>13</v>
       </c>
-      <c r="E19" t="s" s="13">
+      <c r="E19" t="s" s="15">
         <v>88</v>
       </c>
-      <c r="F19" t="s" s="13">
+      <c r="F19" t="s" s="15">
         <v>89</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" t="s" s="13">
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
+      <c r="K19" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="L19" s="16">
+      <c r="L19" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="11">
+      <c r="A20" s="13">
         <v>1</v>
       </c>
-      <c r="B20" t="s" s="17">
+      <c r="B20" t="s" s="19">
         <v>90</v>
       </c>
-      <c r="C20" t="s" s="13">
+      <c r="C20" t="s" s="15">
         <v>91</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="18">
         <v>603</v>
       </c>
-      <c r="E20" t="s" s="13">
+      <c r="E20" t="s" s="15">
         <v>92</v>
       </c>
-      <c r="F20" t="s" s="13">
+      <c r="F20" t="s" s="15">
         <v>93</v>
       </c>
-      <c r="G20" t="s" s="13">
+      <c r="G20" t="s" s="15">
         <v>94</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" t="s" s="18">
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" t="s" s="20">
         <v>90</v>
       </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="16">
+      <c r="K20" s="16"/>
+      <c r="L20" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="11">
+      <c r="A21" s="13">
         <v>2</v>
       </c>
-      <c r="B21" t="s" s="17">
+      <c r="B21" t="s" s="19">
         <v>95</v>
       </c>
-      <c r="C21" t="s" s="13">
+      <c r="C21" t="s" s="15">
         <v>96</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="18">
         <v>603</v>
       </c>
-      <c r="E21" t="s" s="13">
+      <c r="E21" t="s" s="15">
         <v>97</v>
       </c>
-      <c r="F21" t="s" s="13">
+      <c r="F21" t="s" s="15">
         <v>98</v>
       </c>
-      <c r="G21" t="s" s="13">
+      <c r="G21" t="s" s="15">
         <v>99</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="19">
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="21">
         <v>1</v>
       </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="16">
+      <c r="K21" s="16"/>
+      <c r="L21" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="11">
+      <c r="A22" s="13">
         <v>2</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="22">
         <v>22</v>
       </c>
-      <c r="C22" t="s" s="13">
+      <c r="C22" t="s" s="15">
         <v>100</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="18">
         <v>603</v>
       </c>
-      <c r="E22" t="s" s="13">
+      <c r="E22" t="s" s="15">
         <v>101</v>
       </c>
-      <c r="F22" t="s" s="13">
+      <c r="F22" t="s" s="15">
         <v>102</v>
       </c>
-      <c r="G22" t="s" s="13">
+      <c r="G22" t="s" s="15">
         <v>103</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="19">
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="21">
         <v>22</v>
       </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="16">
+      <c r="K22" s="16"/>
+      <c r="L22" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="11">
+      <c r="A23" s="13">
         <v>1</v>
       </c>
-      <c r="B23" t="s" s="17">
+      <c r="B23" t="s" s="19">
         <v>104</v>
       </c>
-      <c r="C23" t="s" s="13">
+      <c r="C23" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D23" t="s" s="13">
+      <c r="D23" t="s" s="15">
         <v>106</v>
       </c>
-      <c r="E23" t="s" s="13">
+      <c r="E23" t="s" s="15">
         <v>107</v>
       </c>
-      <c r="F23" t="s" s="13">
+      <c r="F23" t="s" s="15">
         <v>108</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="16">
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="11">
+      <c r="A24" s="13">
         <v>2</v>
       </c>
-      <c r="B24" s="20">
+      <c r="B24" s="22">
         <v>470</v>
       </c>
-      <c r="C24" t="s" s="13">
+      <c r="C24" t="s" s="15">
         <v>109</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="18">
         <v>603</v>
       </c>
-      <c r="E24" t="s" s="13">
+      <c r="E24" t="s" s="15">
         <v>110</v>
       </c>
-      <c r="F24" t="s" s="13">
+      <c r="F24" t="s" s="15">
         <v>111</v>
       </c>
-      <c r="G24" t="s" s="13">
+      <c r="G24" t="s" s="15">
         <v>112</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="19">
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="21">
         <v>470</v>
       </c>
-      <c r="K24" s="14"/>
-      <c r="L24" s="16">
+      <c r="K24" s="16"/>
+      <c r="L24" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="11">
+      <c r="A25" s="13">
         <v>2</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="22">
         <v>680</v>
       </c>
-      <c r="C25" t="s" s="13">
+      <c r="C25" t="s" s="15">
         <v>113</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="18">
         <v>603</v>
       </c>
-      <c r="E25" t="s" s="13">
+      <c r="E25" t="s" s="15">
         <v>114</v>
       </c>
-      <c r="F25" t="s" s="13">
+      <c r="F25" t="s" s="15">
         <v>115</v>
       </c>
-      <c r="G25" t="s" s="13">
+      <c r="G25" t="s" s="15">
         <v>116</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="19">
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="21">
         <v>680</v>
       </c>
-      <c r="K25" s="14"/>
-      <c r="L25" s="16">
+      <c r="K25" s="16"/>
+      <c r="L25" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="11">
+      <c r="A26" s="13">
         <v>1</v>
       </c>
-      <c r="B26" t="s" s="17">
+      <c r="B26" t="s" s="19">
         <v>117</v>
       </c>
-      <c r="C26" t="s" s="13">
+      <c r="C26" t="s" s="15">
         <v>105</v>
       </c>
-      <c r="D26" t="s" s="13">
+      <c r="D26" t="s" s="15">
         <v>106</v>
       </c>
-      <c r="E26" t="s" s="13">
+      <c r="E26" t="s" s="15">
         <v>118</v>
       </c>
-      <c r="F26" t="s" s="13">
+      <c r="F26" t="s" s="15">
         <v>108</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="16">
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="11">
+      <c r="A27" s="13">
         <v>1</v>
       </c>
-      <c r="B27" t="s" s="17">
+      <c r="B27" t="s" s="19">
         <v>119</v>
       </c>
-      <c r="C27" t="s" s="13">
+      <c r="C27" t="s" s="15">
         <v>120</v>
       </c>
-      <c r="D27" t="s" s="13">
+      <c r="D27" t="s" s="15">
         <v>121</v>
       </c>
-      <c r="E27" t="s" s="13">
+      <c r="E27" t="s" s="15">
         <v>122</v>
       </c>
-      <c r="F27" t="s" s="13">
+      <c r="F27" t="s" s="15">
         <v>123</v>
       </c>
-      <c r="G27" t="s" s="13">
+      <c r="G27" t="s" s="15">
         <v>124</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" t="s" s="18">
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" t="s" s="20">
         <v>119</v>
       </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="16">
+      <c r="K27" s="16"/>
+      <c r="L27" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="11">
+      <c r="A28" s="13">
         <v>2</v>
       </c>
-      <c r="B28" t="s" s="17">
+      <c r="B28" t="s" s="19">
         <v>125</v>
       </c>
-      <c r="C28" t="s" s="13">
+      <c r="C28" t="s" s="15">
         <v>126</v>
       </c>
-      <c r="D28" t="s" s="13">
+      <c r="D28" t="s" s="15">
         <v>127</v>
       </c>
-      <c r="E28" t="s" s="13">
+      <c r="E28" t="s" s="15">
         <v>128</v>
       </c>
-      <c r="F28" t="s" s="13">
+      <c r="F28" t="s" s="15">
         <v>129</v>
       </c>
-      <c r="G28" t="s" s="13">
+      <c r="G28" t="s" s="15">
         <v>130</v>
       </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" t="s" s="18">
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" t="s" s="20">
         <v>125</v>
       </c>
-      <c r="K28" s="14"/>
-      <c r="L28" s="16">
+      <c r="K28" s="16"/>
+      <c r="L28" s="18">
         <f>A2:A31*5</f>
         <v>10</v>
       </c>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" s="11">
+      <c r="A29" s="13">
         <v>1</v>
       </c>
-      <c r="B29" t="s" s="17">
+      <c r="B29" t="s" s="19">
         <v>131</v>
       </c>
-      <c r="C29" t="s" s="13">
+      <c r="C29" t="s" s="15">
         <v>132</v>
       </c>
-      <c r="D29" t="s" s="13">
+      <c r="D29" t="s" s="15">
         <v>133</v>
       </c>
-      <c r="E29" t="s" s="13">
+      <c r="E29" t="s" s="15">
         <v>134</v>
       </c>
-      <c r="F29" t="s" s="13">
+      <c r="F29" t="s" s="15">
         <v>135</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="16">
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" s="11">
+      <c r="A30" s="13">
         <v>1</v>
       </c>
-      <c r="B30" t="s" s="17">
+      <c r="B30" t="s" s="19">
         <v>136</v>
       </c>
-      <c r="C30" t="s" s="13">
+      <c r="C30" t="s" s="15">
         <v>137</v>
       </c>
-      <c r="D30" t="s" s="13">
+      <c r="D30" t="s" s="15">
         <v>138</v>
       </c>
-      <c r="E30" t="s" s="13">
+      <c r="E30" t="s" s="15">
         <v>139</v>
       </c>
-      <c r="F30" t="s" s="13">
+      <c r="F30" t="s" s="15">
         <v>140</v>
       </c>
-      <c r="G30" t="s" s="13">
+      <c r="G30" t="s" s="15">
         <v>141</v>
       </c>
-      <c r="H30" s="14"/>
-      <c r="I30" t="s" s="13">
+      <c r="H30" s="16"/>
+      <c r="I30" t="s" s="15">
         <v>142</v>
       </c>
-      <c r="J30" t="s" s="18">
+      <c r="J30" t="s" s="20">
         <v>143</v>
       </c>
-      <c r="K30" t="s" s="13">
+      <c r="K30" t="s" s="15">
         <v>144</v>
       </c>
-      <c r="L30" s="16">
+      <c r="L30" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>
     </row>
     <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" s="11">
+      <c r="A31" s="13">
         <v>1</v>
       </c>
-      <c r="B31" t="s" s="17">
+      <c r="B31" t="s" s="19">
         <v>145</v>
       </c>
-      <c r="C31" t="s" s="13">
+      <c r="C31" t="s" s="15">
         <v>145</v>
       </c>
-      <c r="D31" t="s" s="13">
+      <c r="D31" t="s" s="15">
         <v>146</v>
       </c>
-      <c r="E31" t="s" s="13">
+      <c r="E31" t="s" s="15">
         <v>147</v>
       </c>
-      <c r="F31" t="s" s="13">
+      <c r="F31" t="s" s="15">
         <v>148</v>
       </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="16">
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="18">
         <f>A2:A31*5</f>
         <v>5</v>
       </c>

</xml_diff>